<commit_message>
updated Planning KW 12
</commit_message>
<xml_diff>
--- a/Planning/KW_12.xlsx
+++ b/Planning/KW_12.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218A3216-5EE0-4DBF-9C96-8F16066EE9C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAE10E3-0482-4CCC-BD5D-72979F321EC7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Task</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>3h</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,6 +418,15 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
@@ -421,6 +436,15 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">

</xml_diff>